<commit_message>
updated table 1 and 2 creation to be via openxlsx with formatting
</commit_message>
<xml_diff>
--- a/Outputs/Tables/T2.xlsx
+++ b/Outputs/Tables/T2.xlsx
@@ -14,6 +14,195 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
+    <t xml:space="preserve">GROUP: Class: Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGROCHEMICALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">161 (36·3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Insecticides and Pesticides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 (50%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Organophosphate*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 (34%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Pyrethroid†</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 (28%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Organochlorine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 (23%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Carbamate‡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 (11%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Synergists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (&lt; 5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Insect Repellents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (&lt; 5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Pyrrole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Herbicides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58 (36%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sulfonylurea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 (17%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Chloroacetanilide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 (14%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Thiocarbamate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Triazine¶</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Phenylurea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Amide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Phenoxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Uracil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Dinitroaniline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Dinitrophenol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (10%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Fungicides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (12%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Azole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (30%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Anilinopyrimidine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (10%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Phthalimide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sulfamide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Plant Growth Regulators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (&lt; 5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTHER CHEMICALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59 (13·3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Flavoring or Fragrance Agents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (53%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Preservatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 (24%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Parabens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 (57%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (43%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Organic UV Filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Pharmacologic Agents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (7%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Emollients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Antioxidants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Humectants</t>
+  </si>
+  <si>
     <t xml:space="preserve">POLLUTANTS AND INDUSTRIAL CHEMICALS</t>
   </si>
   <si>
@@ -32,7 +221,7 @@
     <t xml:space="preserve">37 (17%)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Plasticizers and Plastic Additives‡</t>
+    <t xml:space="preserve">    Plasticizers and Plastic Additives</t>
   </si>
   <si>
     <t xml:space="preserve">27 (12%)</t>
@@ -134,199 +323,10 @@
     <t xml:space="preserve">    Explosive Intermediates</t>
   </si>
   <si>
-    <t xml:space="preserve">3 (&lt; 5%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Disinfectant Breakdown Products</t>
   </si>
   <si>
-    <t xml:space="preserve">2 (&lt; 5%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Side-Reaction Byproducts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (&lt; 5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGROCHEMICALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">161 (36·3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Insecticides and Pesticides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80 (50%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Organophosphate*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 (34%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Pyrethroid†</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 (28%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Organochlorine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 (23%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Carbamate‡</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 (11%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Synergists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Insect Repellents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Pyrrole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Herbicides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58 (36%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Sulfonylurea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 (17%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Chloroacetanilide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 (14%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Thiocarbamate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Triazine¶</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (10%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Phenylurea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Amide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Phenoxy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Uracil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Dinitroaniline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Dinitrophenol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Fungicides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 (12%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Azole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (30%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Anilinopyrimidine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (10%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Phthalimide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Sulfamide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Plant Growth Regulators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTHER CHEMICALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59 (13·3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Flavoring or Fragrance Agents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 (53%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Preservatives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (24%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Parabens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 (57%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (43%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Organic UV Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Pharmacologic Agents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Emollients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Antioxidants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Humectants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n (%)</t>
   </si>
 </sst>
 </file>
@@ -378,16 +378,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,120 +688,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
@@ -809,391 +811,391 @@
         <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B17" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
+    <row r="25">
+      <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>48</v>
+      <c r="B27" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="3" t="s">
+      <c r="B39" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B40" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="4" t="s">
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="s">
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="4" t="s">
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="2" t="s">
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>83</v>
+      <c r="A52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>40</v>
+      <c r="B54" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>88</v>
+      <c r="A55" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>94</v>
+      <c r="A58" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>95</v>
+      <c r="A59" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>